<commit_message>
13-02-2026 commited for changes
</commit_message>
<xml_diff>
--- a/Icaffe_Export Sea_Masters Test Cases.xlsx
+++ b/Icaffe_Export Sea_Masters Test Cases.xlsx
@@ -10277,9 +10277,6 @@
     </r>
   </si>
   <si>
-    <t>User Verify Gst No textbox accepted invalid Gst No.                                                                                                                                                                                                                Note : The same GSTIN validation behavior is implemented and functioning correctly on other pages as well, including Shipline, Shipper, Sub-Agent, IATA Agent, and Vendor Master. The system rejects the GSTIN when the first two digits are correct but the remaining format is invalid.</t>
-  </si>
-  <si>
     <t>Step 1.Navigate icaffe login page
 Step 2.After Login Navigate Login Branch Division
 Step 3.After select Exporter Sea Branch Navigate &gt;Masters&gt;Party&gt;Vendor Master Page                                                                                    Step 4.Click on select drop down in GST St                     Step 5.Select Delhi from drop down field       Step 6.Verify Gst St Code Populated                Step 7.Now enter invalid GSTIN formats one by one.                                                                                      Step 8. Observe whether the system rejects invalid GSTIN numbers and displays validation messages                                                                          Step 9.Click on Add button</t>
@@ -10843,14 +10840,63 @@
 Unwanted characters like @ ! % * ^ &lt; &gt; were accepted in fields where they should be rejected.</t>
   </si>
   <si>
-    <t>When the user enters the first two digits Incorrectly Vendor Invoice add in grid with invalid Gst No. or enters an invalid GSTIN format for the remaining characters, the system accept the incorrect GSTIN format. Actual is not same as expected</t>
+    <r>
+      <t xml:space="preserve">User Verify Gst No textbox accepted invalid Gst No.                                                                                                                                                                                                                Note : The same GSTIN validation behavior is implemented and functioning correctly on other pages as well, including Shipline, Shipper, Sub-Agent, IATA Agent, and Vendor Master. The system rejects the GSTIN when the first two digits are correct but the remaining format is invalid.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: 
+* As per the development team discussion, GSTIN validation is limited to
+* verifying the first two digits (state code) and ensuring a valid 15-digit length.
+* No validation is performed on the remaining characters of the GSTIN.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Shipper Master
+System validates the first two digits (state code) correctly.
+However, if the remaining GSTIN format is invalid, the system still allows save/submit.
+validation message is not displayed and System should reject or display validation message but does not
+Shipline Master
+GSTIN field checks only the initial two digits.
+Invalid GSTIN formats (other than first two digits) are accepted.
+System should reject or display validation message but does not.
+Sub-Agent Master
+System validates the first two digits (state code) correctly.
+However, if the remaining GSTIN format is invalid, the system still allows save/submit.
+validation message is not displayed and System should reject or display validation message but does not
+IATA Agent Master
+System validates the first two digits (state code) correctly.
+However, if the remaining GSTIN format is invalid, the system still allows save/submit.
+validation message is not displayed and System should reject or display validation message but does not
+Vendor Master
+The first two digits (state code) of the GSTIN are different from the selected state code, and
+An invalid GSTIN is entered without completing the required 15 digits.
+The system does not display any validation message for these cases.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10952,6 +10998,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF292A2E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -11065,7 +11125,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11381,12 +11441,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -21885,22 +21939,22 @@
         <v>1543</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>1662</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>1570</v>
       </c>
       <c r="L7" s="9" t="s">
+        <v>2973</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>2974</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>2975</v>
       </c>
       <c r="N7" s="39" t="s">
         <v>2175</v>
@@ -24583,7 +24637,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>22</v>
@@ -24627,7 +24681,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>22</v>
@@ -24671,7 +24725,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>22</v>
@@ -24715,7 +24769,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="C65" s="51" t="s">
         <v>2798</v>
@@ -24780,10 +24834,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>2995</v>
-      </c>
-      <c r="C66" s="128" t="s">
-        <v>2968</v>
+        <v>2994</v>
+      </c>
+      <c r="C66" s="126" t="s">
+        <v>2967</v>
       </c>
       <c r="D66" s="59">
         <v>46031</v>
@@ -24798,22 +24852,22 @@
         <v>1543</v>
       </c>
       <c r="H66" s="53" t="s">
+        <v>2975</v>
+      </c>
+      <c r="I66" s="53" t="s">
         <v>2976</v>
       </c>
-      <c r="I66" s="53" t="s">
+      <c r="J66" s="53" t="s">
+        <v>2965</v>
+      </c>
+      <c r="K66" s="53" t="s">
+        <v>2966</v>
+      </c>
+      <c r="L66" s="53" t="s">
         <v>2977</v>
       </c>
-      <c r="J66" s="53" t="s">
-        <v>2966</v>
-      </c>
-      <c r="K66" s="53" t="s">
-        <v>2967</v>
-      </c>
-      <c r="L66" s="53" t="s">
+      <c r="M66" s="53" t="s">
         <v>2978</v>
-      </c>
-      <c r="M66" s="53" t="s">
-        <v>2979</v>
       </c>
       <c r="N66" s="53" t="s">
         <v>2175</v>
@@ -24825,13 +24879,13 @@
         <v>44205</v>
       </c>
       <c r="Q66" s="52" t="s">
+        <v>2968</v>
+      </c>
+      <c r="R66" s="52" t="s">
         <v>2969</v>
       </c>
-      <c r="R66" s="52" t="s">
+      <c r="S66" s="53" t="s">
         <v>2970</v>
-      </c>
-      <c r="S66" s="53" t="s">
-        <v>2971</v>
       </c>
       <c r="T66" s="59">
         <v>46042</v>
@@ -24845,10 +24899,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>2996</v>
-      </c>
-      <c r="C67" s="128" t="s">
-        <v>2968</v>
+        <v>2995</v>
+      </c>
+      <c r="C67" s="126" t="s">
+        <v>2967</v>
       </c>
       <c r="D67" s="59">
         <v>46031</v>
@@ -24862,23 +24916,23 @@
       <c r="G67" s="52" t="s">
         <v>1543</v>
       </c>
-      <c r="H67" s="130" t="s">
-        <v>2997</v>
+      <c r="H67" s="128" t="s">
+        <v>2996</v>
       </c>
       <c r="I67" s="53" t="s">
+        <v>2988</v>
+      </c>
+      <c r="J67" s="74" t="s">
+        <v>2983</v>
+      </c>
+      <c r="K67" s="127" t="s">
+        <v>209</v>
+      </c>
+      <c r="L67" s="53" t="s">
         <v>2989</v>
       </c>
-      <c r="J67" s="74" t="s">
+      <c r="M67" s="53" t="s">
         <v>2984</v>
-      </c>
-      <c r="K67" s="129" t="s">
-        <v>209</v>
-      </c>
-      <c r="L67" s="53" t="s">
-        <v>2990</v>
-      </c>
-      <c r="M67" s="53" t="s">
-        <v>2985</v>
       </c>
       <c r="N67" s="53" t="s">
         <v>2175</v>
@@ -24890,13 +24944,13 @@
         <v>46031</v>
       </c>
       <c r="Q67" s="49" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="R67" s="49" t="s">
         <v>1024</v>
       </c>
       <c r="S67" s="53" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="T67" s="59">
         <v>46042</v>
@@ -24907,7 +24961,7 @@
     </row>
     <row r="68" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="C68" s="9" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
     </row>
   </sheetData>
@@ -27179,7 +27233,7 @@
         <v>1988</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>1989</v>
@@ -27230,7 +27284,7 @@
         <v>1998</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J3" s="39" t="s">
         <v>1999</v>
@@ -27280,7 +27334,7 @@
         <v>2004</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J4" s="39" t="s">
         <v>2005</v>
@@ -27330,7 +27384,7 @@
         <v>2009</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J5" s="39" t="s">
         <v>2010</v>
@@ -27380,7 +27434,7 @@
         <v>2033</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J6" s="39" t="s">
         <v>2014</v>
@@ -27427,10 +27481,10 @@
         <v>1987</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J7" s="39" t="s">
         <v>2018</v>
@@ -27439,10 +27493,10 @@
         <v>2019</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="M7" s="39" t="s">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="N7" s="39" t="s">
         <v>2175</v>
@@ -27481,7 +27535,7 @@
         <v>2021</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J8" s="39" t="s">
         <v>2027</v>
@@ -27536,7 +27590,7 @@
         <v>2026</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J9" s="53" t="s">
         <v>2028</v>
@@ -27597,7 +27651,7 @@
         <v>2034</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>2035</v>
@@ -27647,7 +27701,7 @@
         <v>2039</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J11" s="41" t="s">
         <v>2040</v>
@@ -27698,7 +27752,7 @@
         <v>2043</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J12" s="41" t="s">
         <v>2044</v>
@@ -27749,7 +27803,7 @@
         <v>2050</v>
       </c>
       <c r="I13" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J13" s="41" t="s">
         <v>2051</v>
@@ -27800,7 +27854,7 @@
         <v>2056</v>
       </c>
       <c r="I14" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J14" s="41" t="s">
         <v>2062</v>
@@ -27855,7 +27909,7 @@
         <v>2061</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>2063</v>
@@ -27916,7 +27970,7 @@
         <v>2075</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J16" s="41" t="s">
         <v>2073</v>
@@ -27967,7 +28021,7 @@
         <v>2076</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J17" s="41" t="s">
         <v>2068</v>
@@ -28016,7 +28070,7 @@
         <v>2078</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J18" s="41" t="s">
         <v>2079</v>
@@ -28061,7 +28115,7 @@
         <v>2084</v>
       </c>
       <c r="I19" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J19" s="41" t="s">
         <v>2085</v>
@@ -28106,7 +28160,7 @@
         <v>2090</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>2091</v>
@@ -28151,7 +28205,7 @@
         <v>2096</v>
       </c>
       <c r="I21" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J21" s="41" t="s">
         <v>2097</v>
@@ -28196,7 +28250,7 @@
         <v>2103</v>
       </c>
       <c r="I22" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J22" s="41" t="s">
         <v>2104</v>
@@ -28241,7 +28295,7 @@
         <v>2108</v>
       </c>
       <c r="I23" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J23" s="41" t="s">
         <v>2109</v>
@@ -28286,7 +28340,7 @@
         <v>2113</v>
       </c>
       <c r="I24" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>2114</v>
@@ -28331,7 +28385,7 @@
         <v>2118</v>
       </c>
       <c r="I25" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J25" s="41" t="s">
         <v>2119</v>
@@ -28376,7 +28430,7 @@
         <v>2127</v>
       </c>
       <c r="I26" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>2109</v>
@@ -28421,7 +28475,7 @@
         <v>2128</v>
       </c>
       <c r="I27" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>2114</v>
@@ -28466,7 +28520,7 @@
         <v>1747</v>
       </c>
       <c r="I28" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J28" s="41" t="s">
         <v>2136</v>
@@ -28517,7 +28571,7 @@
         <v>1753</v>
       </c>
       <c r="I29" s="53" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>2141</v>
@@ -28573,7 +28627,7 @@
         <v>2143</v>
       </c>
       <c r="I30" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J30" s="41" t="s">
         <v>2144</v>
@@ -28620,7 +28674,7 @@
         <v>2148</v>
       </c>
       <c r="I31" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J31" s="41" t="s">
         <v>2149</v>
@@ -28665,7 +28719,7 @@
         <v>416</v>
       </c>
       <c r="I32" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>2152</v>
@@ -28710,7 +28764,7 @@
         <v>2157</v>
       </c>
       <c r="I33" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J33" s="41" t="s">
         <v>2160</v>
@@ -28755,7 +28809,7 @@
         <v>2163</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J34" s="41" t="s">
         <v>2168</v>
@@ -28800,7 +28854,7 @@
         <v>2167</v>
       </c>
       <c r="I35" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J35" s="41" t="s">
         <v>2169</v>
@@ -28845,7 +28899,7 @@
         <v>2176</v>
       </c>
       <c r="I36" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J36" s="41" t="s">
         <v>2188</v>
@@ -28890,7 +28944,7 @@
         <v>2181</v>
       </c>
       <c r="I37" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J37" s="41" t="s">
         <v>2187</v>
@@ -28935,7 +28989,7 @@
         <v>2185</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J38" s="41" t="s">
         <v>2186</v>
@@ -28980,7 +29034,7 @@
         <v>2193</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J39" s="41" t="s">
         <v>2194</v>
@@ -29025,7 +29079,7 @@
         <v>2198</v>
       </c>
       <c r="I40" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J40" s="41" t="s">
         <v>2200</v>
@@ -29055,7 +29109,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>22</v>
@@ -29070,7 +29124,7 @@
         <v>2199</v>
       </c>
       <c r="I41" s="41" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="J41" s="41" t="s">
         <v>2201</v>
@@ -29100,13 +29154,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>2983</v>
-      </c>
-      <c r="C42" s="128" t="s">
-        <v>2968</v>
+        <v>2982</v>
+      </c>
+      <c r="C42" s="126" t="s">
+        <v>2967</v>
       </c>
       <c r="D42" s="59" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="E42" s="49" t="s">
         <v>22</v>
@@ -29118,22 +29172,22 @@
         <v>1987</v>
       </c>
       <c r="H42" s="53" t="s">
+        <v>2979</v>
+      </c>
+      <c r="I42" s="53" t="s">
+        <v>2964</v>
+      </c>
+      <c r="J42" s="53" t="s">
+        <v>2965</v>
+      </c>
+      <c r="K42" s="53" t="s">
+        <v>2966</v>
+      </c>
+      <c r="L42" s="53" t="s">
         <v>2980</v>
       </c>
-      <c r="I42" s="53" t="s">
-        <v>2965</v>
-      </c>
-      <c r="J42" s="53" t="s">
-        <v>2966</v>
-      </c>
-      <c r="K42" s="53" t="s">
-        <v>2967</v>
-      </c>
-      <c r="L42" s="53" t="s">
+      <c r="M42" s="53" t="s">
         <v>2981</v>
-      </c>
-      <c r="M42" s="53" t="s">
-        <v>2982</v>
       </c>
       <c r="N42" s="53" t="s">
         <v>2175</v>
@@ -29145,13 +29199,13 @@
         <v>44205</v>
       </c>
       <c r="Q42" s="52" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="R42" s="52" t="s">
         <v>1024</v>
       </c>
       <c r="S42" s="53" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="T42" s="59">
         <v>46042</v>
@@ -29165,13 +29219,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>2998</v>
-      </c>
-      <c r="C43" s="128" t="s">
-        <v>2968</v>
+        <v>2997</v>
+      </c>
+      <c r="C43" s="126" t="s">
+        <v>2967</v>
       </c>
       <c r="D43" s="59" t="s">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="E43" s="49" t="s">
         <v>22</v>
@@ -29182,23 +29236,23 @@
       <c r="G43" s="49" t="s">
         <v>1987</v>
       </c>
-      <c r="H43" s="130" t="s">
+      <c r="H43" s="128" t="s">
+        <v>2998</v>
+      </c>
+      <c r="I43" s="53" t="s">
         <v>2999</v>
       </c>
-      <c r="I43" s="53" t="s">
-        <v>3000</v>
-      </c>
       <c r="J43" s="74" t="s">
+        <v>2983</v>
+      </c>
+      <c r="K43" s="127" t="s">
+        <v>209</v>
+      </c>
+      <c r="L43" s="53" t="s">
+        <v>2989</v>
+      </c>
+      <c r="M43" s="53" t="s">
         <v>2984</v>
-      </c>
-      <c r="K43" s="129" t="s">
-        <v>209</v>
-      </c>
-      <c r="L43" s="53" t="s">
-        <v>2990</v>
-      </c>
-      <c r="M43" s="53" t="s">
-        <v>2985</v>
       </c>
       <c r="N43" s="53" t="s">
         <v>2175</v>
@@ -29210,13 +29264,13 @@
         <v>46031</v>
       </c>
       <c r="Q43" s="49" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="R43" s="49" t="s">
         <v>1024</v>
       </c>
       <c r="S43" s="53" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="T43" s="59">
         <v>46042</v>
@@ -29227,7 +29281,7 @@
     </row>
     <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="39" t="s">
-        <v>3005</v>
+        <v>3004</v>
       </c>
     </row>
   </sheetData>
@@ -31087,10 +31141,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>3027</v>
-      </c>
-      <c r="C35" s="128" t="s">
-        <v>3010</v>
+        <v>3026</v>
+      </c>
+      <c r="C35" s="126" t="s">
+        <v>3009</v>
       </c>
       <c r="D35" s="54">
         <v>46030</v>
@@ -31105,22 +31159,22 @@
         <v>2208</v>
       </c>
       <c r="H35" s="50" t="s">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="I35" s="53" t="s">
         <v>2209</v>
       </c>
       <c r="J35" s="53" t="s">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="K35" s="50" t="s">
         <v>209</v>
       </c>
       <c r="L35" s="53" t="s">
+        <v>3006</v>
+      </c>
+      <c r="M35" s="53" t="s">
         <v>3007</v>
-      </c>
-      <c r="M35" s="53" t="s">
-        <v>3008</v>
       </c>
       <c r="N35" s="53" t="s">
         <v>38</v>
@@ -31132,16 +31186,16 @@
         <v>46030</v>
       </c>
       <c r="Q35" s="53" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="R35" s="52" t="s">
         <v>1024</v>
       </c>
-      <c r="S35" s="132" t="s">
+      <c r="S35" s="130" t="s">
         <v>2910</v>
       </c>
       <c r="T35" s="59" t="s">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="U35" s="50" t="s">
         <v>1715</v>
@@ -31291,9 +31345,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33306,64 +33360,64 @@
         <v>45924</v>
       </c>
     </row>
-    <row r="44" spans="1:21" s="82" customFormat="1" ht="390" x14ac:dyDescent="0.25">
-      <c r="A44" s="81">
+    <row r="44" spans="1:21" s="52" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="49">
         <v>43</v>
       </c>
-      <c r="B44" s="104" t="s">
+      <c r="B44" s="73" t="s">
         <v>2502</v>
       </c>
-      <c r="C44" s="84" t="s">
+      <c r="C44" s="51" t="s">
         <v>2827</v>
       </c>
-      <c r="D44" s="110">
+      <c r="D44" s="86">
         <v>45925</v>
       </c>
-      <c r="E44" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="82" t="s">
+      <c r="E44" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="52" t="s">
         <v>624</v>
       </c>
-      <c r="G44" s="82" t="s">
+      <c r="G44" s="52" t="s">
         <v>2263</v>
       </c>
-      <c r="H44" s="105" t="s">
+      <c r="H44" s="70" t="s">
+        <v>3031</v>
+      </c>
+      <c r="I44" s="53" t="s">
+        <v>2267</v>
+      </c>
+      <c r="J44" s="50" t="s">
         <v>2926</v>
       </c>
-      <c r="I44" s="40" t="s">
-        <v>2267</v>
-      </c>
-      <c r="J44" s="79" t="s">
-        <v>2927</v>
-      </c>
-      <c r="K44" s="105" t="s">
+      <c r="K44" s="70" t="s">
         <v>2925</v>
       </c>
-      <c r="L44" s="79" t="s">
+      <c r="L44" s="50" t="s">
         <v>2924</v>
       </c>
-      <c r="M44" s="105" t="s">
+      <c r="M44" s="70" t="s">
         <v>3032</v>
       </c>
-      <c r="N44" s="40" t="s">
+      <c r="N44" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="O44" s="79" t="s">
+      <c r="O44" s="50" t="s">
         <v>2415</v>
       </c>
-      <c r="P44" s="80">
+      <c r="P44" s="54">
         <v>45924</v>
       </c>
-      <c r="Q44" s="79" t="s">
-        <v>2960</v>
-      </c>
-      <c r="R44" s="82" t="s">
+      <c r="Q44" s="50" t="s">
+        <v>2959</v>
+      </c>
+      <c r="R44" s="52" t="s">
         <v>2918</v>
       </c>
-      <c r="S44" s="79"/>
-      <c r="T44" s="111"/>
-      <c r="U44" s="79"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="56"/>
+      <c r="U44" s="50"/>
     </row>
     <row r="45" spans="1:21" s="18" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
@@ -34864,7 +34918,7 @@
         <v>45927</v>
       </c>
       <c r="Q76" s="79" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="R76" s="82" t="s">
         <v>2918</v>
@@ -34884,7 +34938,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="104" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="C77" s="84" t="s">
         <v>2849</v>
@@ -34902,13 +34956,13 @@
         <v>2263</v>
       </c>
       <c r="H77" s="79" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="I77" s="79" t="s">
         <v>2267</v>
       </c>
       <c r="J77" s="79" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="K77" s="79" t="s">
         <v>209</v>
@@ -34929,13 +34983,13 @@
         <v>45987</v>
       </c>
       <c r="Q77" s="79" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="R77" s="82" t="s">
         <v>2861</v>
       </c>
       <c r="S77" s="40" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="T77" s="106">
         <v>45999</v>
@@ -34945,7 +34999,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G80" s="133"/>
+      <c r="G80" s="131"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U77"/>
@@ -37200,68 +37254,68 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" s="122" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A23" s="113">
-        <v>22</v>
-      </c>
-      <c r="B23" s="114" t="s">
+    <row r="23" spans="1:21" s="120" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A23" s="111">
+        <v>22</v>
+      </c>
+      <c r="B23" s="112" t="s">
         <v>655</v>
       </c>
-      <c r="C23" s="115" t="s">
+      <c r="C23" s="113" t="s">
         <v>2718</v>
       </c>
-      <c r="D23" s="116">
+      <c r="D23" s="114">
         <v>45892</v>
       </c>
-      <c r="E23" s="114" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="114" t="s">
+      <c r="E23" s="112" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="114" t="s">
+      <c r="G23" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="H23" s="117" t="s">
-        <v>2941</v>
-      </c>
-      <c r="I23" s="117" t="s">
+      <c r="H23" s="115" t="s">
+        <v>2940</v>
+      </c>
+      <c r="I23" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="117" t="s">
+      <c r="J23" s="115" t="s">
         <v>765</v>
       </c>
-      <c r="K23" s="117" t="s">
+      <c r="K23" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="117" t="s">
+      <c r="L23" s="115" t="s">
         <v>766</v>
       </c>
-      <c r="M23" s="117" t="s">
-        <v>2940</v>
-      </c>
-      <c r="N23" s="118" t="s">
+      <c r="M23" s="115" t="s">
+        <v>2939</v>
+      </c>
+      <c r="N23" s="116" t="s">
         <v>1000</v>
       </c>
-      <c r="O23" s="117" t="s">
+      <c r="O23" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="P23" s="119">
+      <c r="P23" s="117">
         <v>45875</v>
       </c>
-      <c r="Q23" s="114" t="s">
+      <c r="Q23" s="112" t="s">
         <v>922</v>
       </c>
-      <c r="R23" s="114" t="s">
+      <c r="R23" s="112" t="s">
         <v>1000</v>
       </c>
-      <c r="S23" s="120" t="s">
+      <c r="S23" s="118" t="s">
         <v>2884</v>
       </c>
-      <c r="T23" s="121" t="s">
+      <c r="T23" s="119" t="s">
         <v>2857</v>
       </c>
-      <c r="U23" s="113">
+      <c r="U23" s="111">
         <v>1</v>
       </c>
     </row>
@@ -39215,7 +39269,7 @@
         <v>32</v>
       </c>
       <c r="H61" s="45" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="I61" s="45" t="s">
         <v>25</v>
@@ -39247,7 +39301,7 @@
       <c r="R61" s="7" t="s">
         <v>1000</v>
       </c>
-      <c r="S61" s="112"/>
+      <c r="S61" s="110"/>
       <c r="T61" s="48" t="s">
         <v>998</v>
       </c>
@@ -39441,13 +39495,13 @@
         <v>1024</v>
       </c>
       <c r="S64" s="61" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="T64" s="59" t="s">
         <v>2856</v>
       </c>
       <c r="U64" s="53" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="210" x14ac:dyDescent="0.25">
@@ -39608,7 +39662,7 @@
         <v>1024</v>
       </c>
       <c r="S67" s="61" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="T67" s="59" t="s">
         <v>2860</v>
@@ -39673,7 +39727,7 @@
         <v>1024</v>
       </c>
       <c r="S68" s="61" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="T68" s="59" t="s">
         <v>2859</v>
@@ -39738,7 +39792,7 @@
         <v>1024</v>
       </c>
       <c r="S69" s="50" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="T69" s="59">
         <v>45923</v>
@@ -39767,13 +39821,13 @@
         <v>32</v>
       </c>
       <c r="H70" s="50" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="I70" s="50" t="s">
         <v>1485</v>
       </c>
       <c r="J70" s="50" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="K70" s="50" t="s">
         <v>209</v>
@@ -39800,13 +39854,13 @@
         <v>1024</v>
       </c>
       <c r="S70" s="53" t="s">
-        <v>3024</v>
+        <v>3023</v>
       </c>
       <c r="T70" s="59" t="s">
-        <v>3023</v>
+        <v>3022</v>
       </c>
       <c r="U70" s="53" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="300" x14ac:dyDescent="0.25">
@@ -39814,10 +39868,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="52" t="s">
-        <v>3026</v>
-      </c>
-      <c r="C71" s="128" t="s">
         <v>3025</v>
+      </c>
+      <c r="C71" s="126" t="s">
+        <v>3024</v>
       </c>
       <c r="D71" s="54">
         <v>46030</v>
@@ -39832,22 +39886,22 @@
         <v>32</v>
       </c>
       <c r="H71" s="50" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="I71" s="39" t="s">
         <v>1485</v>
       </c>
       <c r="J71" s="39" t="s">
+        <v>3015</v>
+      </c>
+      <c r="K71" s="50" t="s">
         <v>3016</v>
       </c>
-      <c r="K71" s="50" t="s">
+      <c r="L71" s="39" t="s">
         <v>3017</v>
       </c>
-      <c r="L71" s="39" t="s">
+      <c r="M71" s="39" t="s">
         <v>3018</v>
-      </c>
-      <c r="M71" s="39" t="s">
-        <v>3019</v>
       </c>
       <c r="N71" s="53" t="s">
         <v>38</v>
@@ -39859,19 +39913,19 @@
         <v>46030</v>
       </c>
       <c r="Q71" s="52" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="R71" s="52" t="s">
         <v>1024</v>
       </c>
       <c r="S71" s="53" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="T71" s="59" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="U71" s="53" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
     </row>
   </sheetData>
@@ -40676,16 +40730,16 @@
         <v>25</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>2943</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>2944</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>2945</v>
       </c>
       <c r="N2" s="39" t="s">
         <v>2175</v>
@@ -40758,7 +40812,7 @@
         <v>204</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>25</v>
@@ -40767,10 +40821,10 @@
         <v>202</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>2956</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>2957</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>2958</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>224</v>
@@ -41028,16 +41082,16 @@
         <v>204</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>346</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>2946</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>2947</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>2948</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>345</v>
@@ -41060,10 +41114,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>3012</v>
-      </c>
-      <c r="C11" s="128" t="s">
-        <v>3014</v>
+        <v>3011</v>
+      </c>
+      <c r="C11" s="126" t="s">
+        <v>3013</v>
       </c>
       <c r="D11" s="54">
         <v>46030</v>
@@ -41078,22 +41132,22 @@
         <v>204</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>3028</v>
+        <v>3027</v>
       </c>
       <c r="I11" s="50" t="s">
         <v>346</v>
       </c>
       <c r="J11" s="50" t="s">
-        <v>3029</v>
+        <v>3028</v>
       </c>
       <c r="K11" s="52" t="s">
         <v>209</v>
       </c>
       <c r="L11" s="50" t="s">
+        <v>3029</v>
+      </c>
+      <c r="M11" s="50" t="s">
         <v>3030</v>
-      </c>
-      <c r="M11" s="50" t="s">
-        <v>3031</v>
       </c>
       <c r="N11" s="53" t="s">
         <v>38</v>
@@ -41105,16 +41159,16 @@
         <v>46030</v>
       </c>
       <c r="Q11" s="52" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="R11" s="52" t="s">
         <v>1024</v>
       </c>
       <c r="S11" s="53" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="T11" s="59" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="U11" s="53" t="s">
         <v>2921</v>
@@ -43166,7 +43220,7 @@
       <c r="M32" s="21"/>
       <c r="N32" s="41"/>
       <c r="O32" s="21"/>
-      <c r="P32" s="127"/>
+      <c r="P32" s="125"/>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D33" s="7"/>
@@ -44883,22 +44937,22 @@
         <v>228</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="I26" s="50" t="s">
         <v>25</v>
       </c>
       <c r="J26" s="50" t="s">
+        <v>2928</v>
+      </c>
+      <c r="K26" s="50" t="s">
         <v>2929</v>
       </c>
-      <c r="K26" s="50" t="s">
+      <c r="L26" s="50" t="s">
+        <v>2931</v>
+      </c>
+      <c r="M26" s="50" t="s">
         <v>2930</v>
-      </c>
-      <c r="L26" s="50" t="s">
-        <v>2932</v>
-      </c>
-      <c r="M26" s="50" t="s">
-        <v>2931</v>
       </c>
       <c r="N26" s="53" t="s">
         <v>2175</v>
@@ -44919,7 +44973,7 @@
         <v>2896</v>
       </c>
       <c r="T26" s="59" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="U26" s="53" t="s">
         <v>1704</v>
@@ -49087,10 +49141,10 @@
         <v>57</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>2988</v>
-      </c>
-      <c r="C62" s="128" t="s">
-        <v>2968</v>
+        <v>2987</v>
+      </c>
+      <c r="C62" s="126" t="s">
+        <v>2967</v>
       </c>
       <c r="D62" s="59">
         <v>46031</v>
@@ -49104,23 +49158,23 @@
       <c r="G62" s="53" t="s">
         <v>510</v>
       </c>
-      <c r="H62" s="130" t="s">
-        <v>3001</v>
+      <c r="H62" s="128" t="s">
+        <v>3000</v>
       </c>
       <c r="I62" s="53" t="s">
         <v>917</v>
       </c>
       <c r="J62" s="74" t="s">
+        <v>2983</v>
+      </c>
+      <c r="K62" s="127" t="s">
+        <v>209</v>
+      </c>
+      <c r="L62" s="53" t="s">
+        <v>3001</v>
+      </c>
+      <c r="M62" s="53" t="s">
         <v>2984</v>
-      </c>
-      <c r="K62" s="129" t="s">
-        <v>209</v>
-      </c>
-      <c r="L62" s="53" t="s">
-        <v>3002</v>
-      </c>
-      <c r="M62" s="53" t="s">
-        <v>2985</v>
       </c>
       <c r="N62" s="53" t="s">
         <v>2175</v>
@@ -49132,13 +49186,13 @@
         <v>46031</v>
       </c>
       <c r="Q62" s="49" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="R62" s="49" t="s">
         <v>1024</v>
       </c>
       <c r="S62" s="53" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="T62" s="59">
         <v>46042</v>
@@ -52222,68 +52276,68 @@
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" s="122" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A15" s="113">
+    <row r="15" spans="1:21" s="120" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" s="111">
         <v>14</v>
       </c>
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="115" t="s">
         <v>1246</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="113" t="s">
         <v>2763</v>
       </c>
-      <c r="D15" s="116">
+      <c r="D15" s="114">
         <v>45903</v>
       </c>
-      <c r="E15" s="114" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="114" t="s">
+      <c r="E15" s="112" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="114" t="s">
+      <c r="G15" s="112" t="s">
         <v>1182</v>
       </c>
-      <c r="H15" s="117" t="s">
+      <c r="H15" s="115" t="s">
         <v>1252</v>
       </c>
-      <c r="I15" s="117" t="s">
+      <c r="I15" s="115" t="s">
         <v>1184</v>
       </c>
-      <c r="J15" s="117" t="s">
+      <c r="J15" s="115" t="s">
         <v>1245</v>
       </c>
-      <c r="K15" s="117" t="s">
+      <c r="K15" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="L15" s="117" t="s">
+      <c r="L15" s="115" t="s">
         <v>1251</v>
       </c>
-      <c r="M15" s="117" t="s">
+      <c r="M15" s="115" t="s">
         <v>1253</v>
       </c>
-      <c r="N15" s="118" t="s">
+      <c r="N15" s="116" t="s">
         <v>1000</v>
       </c>
-      <c r="O15" s="117" t="s">
+      <c r="O15" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="P15" s="123">
+      <c r="P15" s="121">
         <v>45902</v>
       </c>
-      <c r="Q15" s="114" t="s">
+      <c r="Q15" s="112" t="s">
         <v>922</v>
       </c>
-      <c r="R15" s="114" t="s">
+      <c r="R15" s="112" t="s">
         <v>1000</v>
       </c>
-      <c r="S15" s="124" t="s">
+      <c r="S15" s="122" t="s">
         <v>2907</v>
       </c>
-      <c r="T15" s="125" t="s">
-        <v>2943</v>
-      </c>
-      <c r="U15" s="126">
+      <c r="T15" s="123" t="s">
+        <v>2942</v>
+      </c>
+      <c r="U15" s="124">
         <v>1</v>
       </c>
     </row>
@@ -52338,68 +52392,68 @@
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" s="122" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A17" s="113">
+    <row r="17" spans="1:21" s="120" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A17" s="111">
         <v>16</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="115" t="s">
         <v>1260</v>
       </c>
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="113" t="s">
         <v>2764</v>
       </c>
-      <c r="D17" s="116">
+      <c r="D17" s="114">
         <v>45904</v>
       </c>
-      <c r="E17" s="114" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="114" t="s">
+      <c r="E17" s="112" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="114" t="s">
+      <c r="G17" s="112" t="s">
         <v>1182</v>
       </c>
-      <c r="H17" s="117" t="s">
+      <c r="H17" s="115" t="s">
         <v>1261</v>
       </c>
-      <c r="I17" s="117" t="s">
+      <c r="I17" s="115" t="s">
         <v>1184</v>
       </c>
-      <c r="J17" s="117" t="s">
+      <c r="J17" s="115" t="s">
         <v>1262</v>
       </c>
-      <c r="K17" s="117" t="s">
+      <c r="K17" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="L17" s="117" t="s">
+      <c r="L17" s="115" t="s">
         <v>1263</v>
       </c>
-      <c r="M17" s="117" t="s">
+      <c r="M17" s="115" t="s">
         <v>1264</v>
       </c>
-      <c r="N17" s="118" t="s">
+      <c r="N17" s="116" t="s">
         <v>1000</v>
       </c>
-      <c r="O17" s="117" t="s">
+      <c r="O17" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="P17" s="123">
+      <c r="P17" s="121">
         <v>45902</v>
       </c>
-      <c r="Q17" s="114" t="s">
+      <c r="Q17" s="112" t="s">
         <v>922</v>
       </c>
-      <c r="R17" s="114" t="s">
+      <c r="R17" s="112" t="s">
         <v>1000</v>
       </c>
-      <c r="S17" s="124" t="s">
+      <c r="S17" s="122" t="s">
         <v>2907</v>
       </c>
-      <c r="T17" s="125" t="s">
-        <v>2942</v>
-      </c>
-      <c r="U17" s="126">
+      <c r="T17" s="123" t="s">
+        <v>2941</v>
+      </c>
+      <c r="U17" s="124">
         <v>1</v>
       </c>
     </row>
@@ -56610,8 +56664,8 @@
       <c r="U37" s="7"/>
     </row>
     <row r="38" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="C38" s="131" t="s">
-        <v>3003</v>
+      <c r="C38" s="129" t="s">
+        <v>3002</v>
       </c>
       <c r="N38" s="39"/>
     </row>

</xml_diff>